<commit_message>
Added Unsuccessful Forgot Password
</commit_message>
<xml_diff>
--- a/Data/testdata.xlsx
+++ b/Data/testdata.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\robot-scripts\sabongeros\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616481DA-12BE-430C-97AC-EAE6A93FFEB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9A8E95-3F3C-4EC2-B851-FE00816F979F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E7A5B3BB-D570-4591-8F6A-59A139A91B3F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E7A5B3BB-D570-4591-8F6A-59A139A91B3F}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="registration" sheetId="2" r:id="rId2"/>
+    <sheet name="forgotpassword" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="50">
   <si>
     <t>${email}</t>
   </si>
@@ -167,6 +168,15 @@
   </si>
   <si>
     <t>01/01/1991</t>
+  </si>
+  <si>
+    <t>Please enter your email or username</t>
+  </si>
+  <si>
+    <t>Account not existing.</t>
+  </si>
+  <si>
+    <t>nonregistered@citrof.com</t>
   </si>
 </sst>
 </file>
@@ -534,7 +544,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,7 +635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3290C14-D097-4996-8F1F-020D469E6C0B}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -1138,4 +1148,57 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId15"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF7575C3-21C8-4301-8A88-22616E0AEFC3}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{AA412CAE-F8FA-44CB-BFBE-F5B2707865A1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added change password scenarios 2
</commit_message>
<xml_diff>
--- a/Data/testdata.xlsx
+++ b/Data/testdata.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\robot-scripts\sabongeros\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9A8E95-3F3C-4EC2-B851-FE00816F979F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469B44B4-2FA8-4B8D-8E4D-4C9A6EC88350}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E7A5B3BB-D570-4591-8F6A-59A139A91B3F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{E7A5B3BB-D570-4591-8F6A-59A139A91B3F}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="registration" sheetId="2" r:id="rId2"/>
     <sheet name="forgotpassword" sheetId="3" r:id="rId3"/>
+    <sheet name="changepassword" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="59">
   <si>
     <t>${email}</t>
   </si>
@@ -177,6 +178,33 @@
   </si>
   <si>
     <t>nonregistered@citrof.com</t>
+  </si>
+  <si>
+    <t>${newpassword}</t>
+  </si>
+  <si>
+    <t>${confirmpassword}</t>
+  </si>
+  <si>
+    <t>Blank new password</t>
+  </si>
+  <si>
+    <t>Less than 8 characters</t>
+  </si>
+  <si>
+    <t>Test1!</t>
+  </si>
+  <si>
+    <t>This field is required</t>
+  </si>
+  <si>
+    <t>Minimum of 8 digits</t>
+  </si>
+  <si>
+    <t>It must contain at least one lowercase letter, one uppercase letter, one numeric digit, and one special character</t>
+  </si>
+  <si>
+    <t>Password do not match</t>
   </si>
 </sst>
 </file>
@@ -221,11 +249,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1154,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF7575C3-21C8-4301-8A88-22616E0AEFC3}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,4 +1233,93 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D81AD8-5DA5-43EE-A627-6C1A5190A4F4}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" customWidth="1"/>
+    <col min="3" max="3" width="36" customWidth="1"/>
+    <col min="4" max="4" width="102.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added edit profile scenarios
</commit_message>
<xml_diff>
--- a/Data/testdata.xlsx
+++ b/Data/testdata.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\robot-scripts\sabongeros\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469B44B4-2FA8-4B8D-8E4D-4C9A6EC88350}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322BF3B1-9EAB-48F0-9381-4858B81FA703}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{E7A5B3BB-D570-4591-8F6A-59A139A91B3F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{E7A5B3BB-D570-4591-8F6A-59A139A91B3F}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="registration" sheetId="2" r:id="rId2"/>
     <sheet name="forgotpassword" sheetId="3" r:id="rId3"/>
     <sheet name="changepassword" sheetId="4" r:id="rId4"/>
+    <sheet name="editprofile" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="75">
   <si>
     <t>${email}</t>
   </si>
@@ -205,13 +206,61 @@
   </si>
   <si>
     <t>Password do not match</t>
+  </si>
+  <si>
+    <t>${firstname}</t>
+  </si>
+  <si>
+    <t>${lastname}</t>
+  </si>
+  <si>
+    <t>${bday}</t>
+  </si>
+  <si>
+    <t>Blank mobile number</t>
+  </si>
+  <si>
+    <t>Username already used</t>
+  </si>
+  <si>
+    <t>Email already used</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>stevemax</t>
+  </si>
+  <si>
+    <t>stevemax@citrof.com</t>
+  </si>
+  <si>
+    <t>01/01/1990</t>
+  </si>
+  <si>
+    <t>Steve</t>
+  </si>
+  <si>
+    <t>stevemax@citrof</t>
+  </si>
+  <si>
+    <t>Invalid input</t>
+  </si>
+  <si>
+    <t>Email already exists</t>
+  </si>
+  <si>
+    <t>Invalid request.</t>
+  </si>
+  <si>
+    <t>jovani.ogaya</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,6 +272,20 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF080808"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -249,7 +312,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -258,6 +321,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1239,9 +1307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D81AD8-5DA5-43EE-A627-6C1A5190A4F4}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1322,4 +1388,336 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7784D03-6FA7-4A94-90E9-5CBF26FE672D}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" customWidth="1"/>
+    <col min="8" max="8" width="34.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2">
+        <v>9221244785</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3">
+        <v>9221244785</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4">
+        <v>9221244785</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5">
+        <v>9221244785</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7">
+        <v>9221244785</v>
+      </c>
+      <c r="H7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8">
+        <v>9221244785</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9">
+        <v>9221244785</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10">
+        <v>9221244785</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11">
+        <v>9221244785</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <v>9221244785</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{4DEE3918-7BEB-450F-89F0-ACCDB0ACF05C}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{5CE35689-0D10-4942-9FA2-42B4E18FAA84}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{F6EE0CCF-7A54-4028-8BF4-CEAFF6A5E2D9}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{C2878E3B-F5D5-4B4E-9741-B5ACFBF45382}"/>
+    <hyperlink ref="E7" r:id="rId5" xr:uid="{35DD3586-C900-4A12-9CAE-2990E4F2F719}"/>
+    <hyperlink ref="E8" r:id="rId6" xr:uid="{B63A8CF0-C5CE-4AD2-ADD8-E4BD6FD58BA2}"/>
+    <hyperlink ref="E9" r:id="rId7" xr:uid="{28FC330F-FC0E-4098-8942-E8DDDCA78464}"/>
+    <hyperlink ref="E10" r:id="rId8" xr:uid="{7DA74E22-E53E-4CBA-82E9-E6FF1A72825A}"/>
+    <hyperlink ref="E11" r:id="rId9" xr:uid="{67DD48A8-0EEC-41E5-A57E-94291009E0CA}"/>
+    <hyperlink ref="E12" r:id="rId10" xr:uid="{5F91BF93-4ADD-435B-BBBF-698C5F630B70}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added cash out scenarios
</commit_message>
<xml_diff>
--- a/Data/testdata.xlsx
+++ b/Data/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\robot-scripts\sabongeros\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322BF3B1-9EAB-48F0-9381-4858B81FA703}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF0742E-0819-4F47-858C-634C4FFA401C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{E7A5B3BB-D570-4591-8F6A-59A139A91B3F}"/>
+    <workbookView xWindow="10125" yWindow="4215" windowWidth="12450" windowHeight="9825" activeTab="4" xr2:uid="{E7A5B3BB-D570-4591-8F6A-59A139A91B3F}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="69">
   <si>
     <t>${email}</t>
   </si>
@@ -217,15 +217,6 @@
     <t>${bday}</t>
   </si>
   <si>
-    <t>Blank mobile number</t>
-  </si>
-  <si>
-    <t>Username already used</t>
-  </si>
-  <si>
-    <t>Email already used</t>
-  </si>
-  <si>
     <t>Max</t>
   </si>
   <si>
@@ -245,15 +236,6 @@
   </si>
   <si>
     <t>Invalid input</t>
-  </si>
-  <si>
-    <t>Email already exists</t>
-  </si>
-  <si>
-    <t>Invalid request.</t>
-  </si>
-  <si>
-    <t>jovani.ogaya</t>
   </si>
 </sst>
 </file>
@@ -1392,10 +1374,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7784D03-6FA7-4A94-90E9-5CBF26FE672D}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1438,13 +1420,16 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>67</v>
@@ -1453,271 +1438,71 @@
         <v>9221244785</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="H2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F3">
         <v>9221244785</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H3" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>62</v>
+      </c>
+      <c r="D4" t="s">
+        <v>63</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F4">
         <v>9221244785</v>
       </c>
       <c r="G4" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="H4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5">
-        <v>9221244785</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F7">
-        <v>9221244785</v>
-      </c>
-      <c r="H7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8">
-        <v>9221244785</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9">
-        <v>9221244785</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F10">
-        <v>9221244785</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11">
-        <v>9221244785</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12">
-        <v>9221244785</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H12" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{4DEE3918-7BEB-450F-89F0-ACCDB0ACF05C}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{5CE35689-0D10-4942-9FA2-42B4E18FAA84}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{F6EE0CCF-7A54-4028-8BF4-CEAFF6A5E2D9}"/>
-    <hyperlink ref="E6" r:id="rId4" xr:uid="{C2878E3B-F5D5-4B4E-9741-B5ACFBF45382}"/>
-    <hyperlink ref="E7" r:id="rId5" xr:uid="{35DD3586-C900-4A12-9CAE-2990E4F2F719}"/>
-    <hyperlink ref="E8" r:id="rId6" xr:uid="{B63A8CF0-C5CE-4AD2-ADD8-E4BD6FD58BA2}"/>
-    <hyperlink ref="E9" r:id="rId7" xr:uid="{28FC330F-FC0E-4098-8942-E8DDDCA78464}"/>
-    <hyperlink ref="E10" r:id="rId8" xr:uid="{7DA74E22-E53E-4CBA-82E9-E6FF1A72825A}"/>
-    <hyperlink ref="E11" r:id="rId9" xr:uid="{67DD48A8-0EEC-41E5-A57E-94291009E0CA}"/>
-    <hyperlink ref="E12" r:id="rId10" xr:uid="{5F91BF93-4ADD-435B-BBBF-698C5F630B70}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{B63A8CF0-C5CE-4AD2-ADD8-E4BD6FD58BA2}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{28FC330F-FC0E-4098-8942-E8DDDCA78464}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{7DA74E22-E53E-4CBA-82E9-E6FF1A72825A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>